<commit_message>
Räknat ut andel vatten och myr runt lyor för alla lyor ink Blankan och Norr Vaktklumpen. Gjort klart distans-sampling skript för stunden i alla fall och printat ut filer. Ändrat myr_sverige_norge-shapefilen till sweref. Lagt till höjd över havet för Blankan och Norr VAktklumpen. Pillat med riptransektfilerna i excel. Tagit bort "m" (meter) bakom alla observationer ur "Höjd"-kolumnen på en av filerna (vilken?). Gjort en ny fil med modifierade ripskitsavstånd för dubbla höger (+10cm) för den ena av dubletter.
</commit_message>
<xml_diff>
--- a/Rawdata/lyor_hojd_helags.xlsx
+++ b/Rawdata/lyor_hojd_helags.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="900" windowWidth="25440" windowHeight="14080" xr2:uid="{22BDC67E-48B9-0E40-A35E-E00D8E23D828}"/>
+    <workbookView xWindow="2260" yWindow="1180" windowWidth="25440" windowHeight="14080" xr2:uid="{22BDC67E-48B9-0E40-A35E-E00D8E23D828}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
   <si>
     <t>Namn</t>
   </si>
@@ -495,6 +495,18 @@
   </si>
   <si>
     <t>hojd_over_havet</t>
+  </si>
+  <si>
+    <t>FSZZ108</t>
+  </si>
+  <si>
+    <t>FSZZ106</t>
+  </si>
+  <si>
+    <t>917.19</t>
+  </si>
+  <si>
+    <t>1078.19</t>
   </si>
 </sst>
 </file>
@@ -846,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13FF60A0-AAB3-3E48-91EA-EBEE591B957A}">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1486,6 +1498,22 @@
         <v>24</v>
       </c>
     </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" t="s">
+        <v>160</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:F79">
     <sortCondition ref="B1"/>

</xml_diff>